<commit_message>
created Overview Page, Your Cart Page, Checkout Page
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/sauceDemo.xlsx
+++ b/src/test/java/TestData/sauceDemo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghost/Downloads/automation/sauceDemo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghost/Downloads/automation/sauceDemo/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{394826EA-F5FB-D247-9BC1-7D4D402639C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743CAA22-B671-7B4B-A2ED-62BF8EC64045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9100" yWindow="-20620" windowWidth="28040" windowHeight="17440" xr2:uid="{D4F29824-6EDE-E149-BE81-EDA3602B3AE4}"/>
+    <workbookView xWindow="-9100" yWindow="-20620" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D4F29824-6EDE-E149-BE81-EDA3602B3AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -78,13 +78,43 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>2191</t>
+  </si>
+  <si>
+    <t>1894</t>
+  </si>
+  <si>
+    <t>2001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +124,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -119,9 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16CA8EF-924A-0946-A805-595268209453}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -511,12 +549,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F72541-502A-484B-81F8-88471FA37AEB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>